<commit_message>
splitted excel files fixed
</commit_message>
<xml_diff>
--- a/not augmented data/differential pressure.xlsx
+++ b/not augmented data/differential pressure.xlsx
@@ -390,13 +390,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D212"/>
+  <dimension ref="A1:D180"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:D212"/>
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.28515625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
@@ -414,13 +420,13 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>992000</v>
+        <v>32988000</v>
       </c>
       <c r="B2" s="1">
-        <v>1.6699581999999999</v>
+        <v>0.21329413</v>
       </c>
       <c r="C2" s="1">
-        <v>1.6699581999999999</v>
+        <v>0.21329413</v>
       </c>
       <c r="D2" s="1">
         <v>12.404602000000001</v>
@@ -428,13 +434,13 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>2000000</v>
+        <v>33992000</v>
       </c>
       <c r="B3" s="1">
-        <v>-0.64994980000000002</v>
+        <v>0.90078365999999999</v>
       </c>
       <c r="C3" s="1">
-        <v>-0.64994980000000002</v>
+        <v>0.90078365999999999</v>
       </c>
       <c r="D3" s="1">
         <v>12.404602000000001</v>
@@ -442,2927 +448,2479 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <v>2988000</v>
+        <v>35000000</v>
       </c>
       <c r="B4" s="1">
-        <v>-1.0243943</v>
+        <v>220.49947</v>
       </c>
       <c r="C4" s="1">
-        <v>-1.0243943</v>
+        <v>220.49947</v>
       </c>
       <c r="D4" s="1">
-        <v>12.404602000000001</v>
+        <v>12.404510500000001</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <v>3996000</v>
+        <v>35984000</v>
       </c>
       <c r="B5" s="1">
-        <v>2.6917903000000001</v>
+        <v>334.82666</v>
       </c>
       <c r="C5" s="1">
-        <v>2.6917903000000001</v>
+        <v>334.82666</v>
       </c>
       <c r="D5" s="1">
-        <v>12.404602000000001</v>
+        <v>12.401337</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
-        <v>5000000</v>
+        <v>36992000</v>
       </c>
       <c r="B6" s="1">
-        <v>1.0514581000000001</v>
+        <v>325.19080000000002</v>
       </c>
       <c r="C6" s="1">
-        <v>1.0514581000000001</v>
+        <v>325.19080000000002</v>
       </c>
       <c r="D6" s="1">
-        <v>12.404602000000001</v>
+        <v>12.37973</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <v>5988000</v>
+        <v>38000000</v>
       </c>
       <c r="B7" s="1">
-        <v>0.24372914000000001</v>
+        <v>314.23108000000002</v>
       </c>
       <c r="C7" s="1">
-        <v>0.24372914000000001</v>
+        <v>314.23108000000002</v>
       </c>
       <c r="D7" s="1">
-        <v>12.404602000000001</v>
+        <v>12.339142000000001</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
-        <v>6992000</v>
+        <v>38984000</v>
       </c>
       <c r="B8" s="1">
-        <v>0.57017899999999999</v>
+        <v>275.25497000000001</v>
       </c>
       <c r="C8" s="1">
-        <v>0.57017899999999999</v>
+        <v>275.25497000000001</v>
       </c>
       <c r="D8" s="1">
-        <v>12.404602000000001</v>
+        <v>12.297302</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
-        <v>8000000</v>
+        <v>39992000</v>
       </c>
       <c r="B9" s="1">
-        <v>-0.15905680999999999</v>
+        <v>270.57816000000003</v>
       </c>
       <c r="C9" s="1">
-        <v>-0.15905680999999999</v>
+        <v>270.57816000000003</v>
       </c>
       <c r="D9" s="1">
-        <v>12.404602000000001</v>
+        <v>12.262421</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <v>8984000</v>
+        <v>41000000</v>
       </c>
       <c r="B10" s="1">
-        <v>-1.553687</v>
+        <v>263.71825999999999</v>
       </c>
       <c r="C10" s="1">
-        <v>-1.553687</v>
+        <v>263.71825999999999</v>
       </c>
       <c r="D10" s="1">
-        <v>12.404602000000001</v>
+        <v>12.229034</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
-        <v>9992000</v>
+        <v>41984000</v>
       </c>
       <c r="B11" s="1">
-        <v>-3.3840286999999997E-2</v>
+        <v>255.21483000000001</v>
       </c>
       <c r="C11" s="1">
-        <v>-3.3840286999999997E-2</v>
+        <v>255.21483000000001</v>
       </c>
       <c r="D11" s="1">
-        <v>12.404602000000001</v>
+        <v>12.196899</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
-        <v>10976000</v>
+        <v>42992000</v>
       </c>
       <c r="B12" s="1">
-        <v>1.7345596999999999</v>
+        <v>249.74768</v>
       </c>
       <c r="C12" s="1">
-        <v>1.7345596999999999</v>
+        <v>249.74768</v>
       </c>
       <c r="D12" s="1">
-        <v>12.404602000000001</v>
+        <v>12.164673000000001</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
-        <v>11984000</v>
+        <v>44000000</v>
       </c>
       <c r="B13" s="1">
-        <v>-0.61978420000000001</v>
+        <v>248.22261</v>
       </c>
       <c r="C13" s="1">
-        <v>-0.61978420000000001</v>
+        <v>248.22261</v>
       </c>
       <c r="D13" s="1">
-        <v>12.404602000000001</v>
+        <v>12.133300999999999</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
-        <v>12992000</v>
+        <v>44984000</v>
       </c>
       <c r="B14" s="1">
-        <v>-7.2501615000000005E-2</v>
+        <v>251.73328000000001</v>
       </c>
       <c r="C14" s="1">
-        <v>-7.2501615000000005E-2</v>
+        <v>251.73328000000001</v>
       </c>
       <c r="D14" s="1">
-        <v>12.404602000000001</v>
+        <v>12.103699000000001</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
-        <v>14000000</v>
+        <v>45992000</v>
       </c>
       <c r="B15" s="1">
-        <v>-0.5278486</v>
+        <v>250.88692</v>
       </c>
       <c r="C15" s="1">
-        <v>-0.5278486</v>
+        <v>250.88692</v>
       </c>
       <c r="D15" s="1">
-        <v>12.404602000000001</v>
+        <v>12.073119999999999</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
-        <v>14984000</v>
+        <v>47000000</v>
       </c>
       <c r="B16" s="1">
-        <v>0.58936480000000002</v>
+        <v>245.97807</v>
       </c>
       <c r="C16" s="1">
-        <v>0.58936480000000002</v>
+        <v>245.97807</v>
       </c>
       <c r="D16" s="1">
-        <v>12.404602000000001</v>
+        <v>12.042419000000001</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
-        <v>15996000</v>
+        <v>47984000</v>
       </c>
       <c r="B17" s="1">
-        <v>1.0664643</v>
+        <v>245.23846</v>
       </c>
       <c r="C17" s="1">
-        <v>1.0664643</v>
+        <v>245.23846</v>
       </c>
       <c r="D17" s="1">
-        <v>12.404602000000001</v>
+        <v>12.012482</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
-        <v>17000000</v>
+        <v>48992000</v>
       </c>
       <c r="B18" s="1">
-        <v>-0.50768535999999997</v>
+        <v>239.78967</v>
       </c>
       <c r="C18" s="1">
-        <v>-0.50768535999999997</v>
+        <v>239.78967</v>
       </c>
       <c r="D18" s="1">
-        <v>12.404602000000001</v>
+        <v>11.981719999999999</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
-        <v>17988000</v>
+        <v>50000000</v>
       </c>
       <c r="B19" s="1">
-        <v>0.69152720000000001</v>
+        <v>238.55823000000001</v>
       </c>
       <c r="C19" s="1">
-        <v>0.69152720000000001</v>
+        <v>238.55823000000001</v>
       </c>
       <c r="D19" s="1">
-        <v>12.404602000000001</v>
+        <v>11.950867000000001</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
-        <v>18992000</v>
+        <v>50984000</v>
       </c>
       <c r="B20" s="1">
-        <v>-0.49217012999999998</v>
+        <v>235.32011</v>
       </c>
       <c r="C20" s="1">
-        <v>-0.49217012999999998</v>
+        <v>235.32011</v>
       </c>
       <c r="D20" s="1">
-        <v>12.404602000000001</v>
+        <v>11.920685000000001</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
-        <v>20004000</v>
+        <v>51992000</v>
       </c>
       <c r="B21" s="1">
-        <v>-0.61180126999999995</v>
+        <v>231.21591000000001</v>
       </c>
       <c r="C21" s="1">
-        <v>-0.61180126999999995</v>
+        <v>231.21591000000001</v>
       </c>
       <c r="D21" s="1">
-        <v>12.404602000000001</v>
+        <v>11.889647999999999</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
-        <v>20984000</v>
+        <v>53000000</v>
       </c>
       <c r="B22" s="1">
-        <v>-0.59901183999999996</v>
+        <v>227.97833</v>
       </c>
       <c r="C22" s="1">
-        <v>-0.59901183999999996</v>
+        <v>227.97833</v>
       </c>
       <c r="D22" s="1">
-        <v>12.404602000000001</v>
+        <v>11.858428999999999</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
-        <v>21992000</v>
+        <v>53988000</v>
       </c>
       <c r="B23" s="1">
-        <v>1.2754037</v>
+        <v>227.08896999999999</v>
       </c>
       <c r="C23" s="1">
-        <v>1.2754037</v>
+        <v>227.08896999999999</v>
       </c>
       <c r="D23" s="1">
-        <v>12.404602000000001</v>
+        <v>11.827728</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
-        <v>23000000</v>
+        <v>54992000</v>
       </c>
       <c r="B24" s="1">
-        <v>1.7193699</v>
+        <v>223.51626999999999</v>
       </c>
       <c r="C24" s="1">
-        <v>1.7193699</v>
+        <v>223.51626999999999</v>
       </c>
       <c r="D24" s="1">
-        <v>12.404602000000001</v>
+        <v>11.796143000000001</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
-        <v>23984000</v>
+        <v>56000000</v>
       </c>
       <c r="B25" s="1">
-        <v>0.94817779999999996</v>
+        <v>219.22086999999999</v>
       </c>
       <c r="C25" s="1">
-        <v>0.94817779999999996</v>
+        <v>219.22086999999999</v>
       </c>
       <c r="D25" s="1">
-        <v>12.404602000000001</v>
+        <v>11.764435000000001</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
-        <v>24992000</v>
+        <v>56984000</v>
       </c>
       <c r="B26" s="1">
-        <v>1.6892138000000001</v>
+        <v>179.42106999999999</v>
       </c>
       <c r="C26" s="1">
-        <v>1.6892138000000001</v>
+        <v>179.42106999999999</v>
       </c>
       <c r="D26" s="1">
-        <v>12.404602000000001</v>
+        <v>11.738007</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
-        <v>26000000</v>
+        <v>57992000</v>
       </c>
       <c r="B27" s="1">
-        <v>0.25881776000000001</v>
+        <v>155.28044</v>
       </c>
       <c r="C27" s="1">
-        <v>0.25881776000000001</v>
+        <v>155.28044</v>
       </c>
       <c r="D27" s="1">
-        <v>12.404602000000001</v>
+        <v>11.729309000000001</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
-        <v>26984000</v>
+        <v>59000000</v>
       </c>
       <c r="B28" s="1">
-        <v>0.93969685000000003</v>
+        <v>148.59575000000001</v>
       </c>
       <c r="C28" s="1">
-        <v>0.93969685000000003</v>
+        <v>148.59575000000001</v>
       </c>
       <c r="D28" s="1">
-        <v>12.404602000000001</v>
+        <v>11.730835000000001</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
-        <v>27996000</v>
+        <v>59984000</v>
       </c>
       <c r="B29" s="1">
-        <v>-1.0232466</v>
+        <v>149.46073999999999</v>
       </c>
       <c r="C29" s="1">
-        <v>-1.0232466</v>
+        <v>149.46073999999999</v>
       </c>
       <c r="D29" s="1">
-        <v>12.404602000000001</v>
+        <v>11.735412999999999</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
-        <v>29000000</v>
+        <v>60992000</v>
       </c>
       <c r="B30" s="1">
-        <v>-0.43228632</v>
+        <v>150.70625000000001</v>
       </c>
       <c r="C30" s="1">
-        <v>-0.43228632</v>
+        <v>150.70625000000001</v>
       </c>
       <c r="D30" s="1">
-        <v>12.404602000000001</v>
+        <v>11.740662</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
-        <v>29988000</v>
+        <v>61999999</v>
       </c>
       <c r="B31" s="1">
-        <v>-1.0381845000000001</v>
+        <v>155.40233000000001</v>
       </c>
       <c r="C31" s="1">
-        <v>-1.0381845000000001</v>
+        <v>155.40233000000001</v>
       </c>
       <c r="D31" s="1">
-        <v>12.404602000000001</v>
+        <v>11.746703999999999</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
-        <v>30992000</v>
+        <v>62984000</v>
       </c>
       <c r="B32" s="1">
-        <v>-0.73986786999999998</v>
+        <v>159.06612000000001</v>
       </c>
       <c r="C32" s="1">
-        <v>-0.73986786999999998</v>
+        <v>159.06612000000001</v>
       </c>
       <c r="D32" s="1">
-        <v>12.404602000000001</v>
+        <v>11.754028</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
-        <v>32000000</v>
+        <v>63992000</v>
       </c>
       <c r="B33" s="1">
-        <v>1.1699046</v>
+        <v>164.63660999999999</v>
       </c>
       <c r="C33" s="1">
-        <v>1.1699046</v>
+        <v>164.63660999999999</v>
       </c>
       <c r="D33" s="1">
-        <v>12.404602000000001</v>
+        <v>11.762207</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
-        <v>32988000</v>
+        <v>65004000</v>
       </c>
       <c r="B34" s="1">
-        <v>0.21329413</v>
+        <v>163.52919</v>
       </c>
       <c r="C34" s="1">
-        <v>0.21329413</v>
+        <v>163.52919</v>
       </c>
       <c r="D34" s="1">
-        <v>12.404602000000001</v>
+        <v>11.767029000000001</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
-        <v>33992000</v>
+        <v>65984000</v>
       </c>
       <c r="B35" s="1">
-        <v>0.90078365999999999</v>
+        <v>152.57642999999999</v>
       </c>
       <c r="C35" s="1">
-        <v>0.90078365999999999</v>
+        <v>152.57642999999999</v>
       </c>
       <c r="D35" s="1">
-        <v>12.404602000000001</v>
+        <v>11.765533</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
-        <v>35000000</v>
+        <v>66992000</v>
       </c>
       <c r="B36" s="1">
-        <v>220.49947</v>
+        <v>141.30330000000001</v>
       </c>
       <c r="C36" s="1">
-        <v>220.49947</v>
+        <v>141.30330000000001</v>
       </c>
       <c r="D36" s="1">
-        <v>12.404510500000001</v>
+        <v>11.760192999999999</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
-        <v>35984000</v>
+        <v>68000000</v>
       </c>
       <c r="B37" s="1">
-        <v>334.82666</v>
+        <v>134.60624999999999</v>
       </c>
       <c r="C37" s="1">
-        <v>334.82666</v>
+        <v>134.60624999999999</v>
       </c>
       <c r="D37" s="1">
-        <v>12.401337</v>
+        <v>11.755646</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
-        <v>36992000</v>
+        <v>68984000</v>
       </c>
       <c r="B38" s="1">
-        <v>325.19080000000002</v>
+        <v>133.74315999999999</v>
       </c>
       <c r="C38" s="1">
-        <v>325.19080000000002</v>
+        <v>133.74315999999999</v>
       </c>
       <c r="D38" s="1">
-        <v>12.37973</v>
+        <v>11.753876</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
-        <v>38000000</v>
+        <v>69992000</v>
       </c>
       <c r="B39" s="1">
-        <v>314.23108000000002</v>
+        <v>133.22400999999999</v>
       </c>
       <c r="C39" s="1">
-        <v>314.23108000000002</v>
+        <v>133.22400999999999</v>
       </c>
       <c r="D39" s="1">
-        <v>12.339142000000001</v>
+        <v>11.75412</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
-        <v>38984000</v>
+        <v>71000000</v>
       </c>
       <c r="B40" s="1">
-        <v>275.25497000000001</v>
+        <v>132.66460000000001</v>
       </c>
       <c r="C40" s="1">
-        <v>275.25497000000001</v>
+        <v>132.66460000000001</v>
       </c>
       <c r="D40" s="1">
-        <v>12.297302</v>
+        <v>11.755065999999999</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
-        <v>39992000</v>
+        <v>71984000</v>
       </c>
       <c r="B41" s="1">
-        <v>270.57816000000003</v>
+        <v>135.80251999999999</v>
       </c>
       <c r="C41" s="1">
-        <v>270.57816000000003</v>
+        <v>135.80251999999999</v>
       </c>
       <c r="D41" s="1">
-        <v>12.262421</v>
+        <v>11.755675999999999</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
-        <v>41000000</v>
+        <v>72992000</v>
       </c>
       <c r="B42" s="1">
-        <v>263.71825999999999</v>
+        <v>135.98079000000001</v>
       </c>
       <c r="C42" s="1">
-        <v>263.71825999999999</v>
+        <v>135.98079000000001</v>
       </c>
       <c r="D42" s="1">
-        <v>12.229034</v>
+        <v>11.755737</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
-        <v>41984000</v>
+        <v>74000000</v>
       </c>
       <c r="B43" s="1">
-        <v>255.21483000000001</v>
+        <v>176.97640000000001</v>
       </c>
       <c r="C43" s="1">
-        <v>255.21483000000001</v>
+        <v>176.97640000000001</v>
       </c>
       <c r="D43" s="1">
-        <v>12.196899</v>
+        <v>11.756378</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
-        <v>42992000</v>
+        <v>74984000</v>
       </c>
       <c r="B44" s="1">
-        <v>249.74768</v>
+        <v>189.58678</v>
       </c>
       <c r="C44" s="1">
-        <v>249.74768</v>
+        <v>189.58678</v>
       </c>
       <c r="D44" s="1">
-        <v>12.164673000000001</v>
+        <v>11.754822000000001</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
-        <v>44000000</v>
+        <v>75992000</v>
       </c>
       <c r="B45" s="1">
-        <v>248.22261</v>
+        <v>166.44802999999999</v>
       </c>
       <c r="C45" s="1">
-        <v>248.22261</v>
+        <v>166.44802999999999</v>
       </c>
       <c r="D45" s="1">
-        <v>12.133300999999999</v>
+        <v>11.753204</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
-        <v>44984000</v>
+        <v>77000000</v>
       </c>
       <c r="B46" s="1">
-        <v>251.73328000000001</v>
+        <v>140.12845999999999</v>
       </c>
       <c r="C46" s="1">
-        <v>251.73328000000001</v>
+        <v>140.12845999999999</v>
       </c>
       <c r="D46" s="1">
-        <v>12.103699000000001</v>
+        <v>11.760223</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
-        <v>45992000</v>
+        <v>77984000</v>
       </c>
       <c r="B47" s="1">
-        <v>250.88692</v>
+        <v>140.74431999999999</v>
       </c>
       <c r="C47" s="1">
-        <v>250.88692</v>
+        <v>140.74431999999999</v>
       </c>
       <c r="D47" s="1">
-        <v>12.073119999999999</v>
+        <v>11.780120999999999</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
-        <v>47000000</v>
+        <v>78992000</v>
       </c>
       <c r="B48" s="1">
-        <v>245.97807</v>
+        <v>147.29279</v>
       </c>
       <c r="C48" s="1">
-        <v>245.97807</v>
+        <v>147.29279</v>
       </c>
       <c r="D48" s="1">
-        <v>12.042419000000001</v>
+        <v>11.806854</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
-        <v>47984000</v>
+        <v>80000000</v>
       </c>
       <c r="B49" s="1">
-        <v>245.23846</v>
+        <v>153.44956999999999</v>
       </c>
       <c r="C49" s="1">
-        <v>245.23846</v>
+        <v>153.44956999999999</v>
       </c>
       <c r="D49" s="1">
-        <v>12.012482</v>
+        <v>11.832336</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
-        <v>48992000</v>
+        <v>80984000</v>
       </c>
       <c r="B50" s="1">
-        <v>239.78967</v>
+        <v>156.43575000000001</v>
       </c>
       <c r="C50" s="1">
-        <v>239.78967</v>
+        <v>156.43575000000001</v>
       </c>
       <c r="D50" s="1">
-        <v>11.981719999999999</v>
+        <v>11.855164</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
-        <v>50000000</v>
+        <v>81992000</v>
       </c>
       <c r="B51" s="1">
-        <v>238.55823000000001</v>
+        <v>151.44386</v>
       </c>
       <c r="C51" s="1">
-        <v>238.55823000000001</v>
+        <v>151.44386</v>
       </c>
       <c r="D51" s="1">
-        <v>11.950867000000001</v>
+        <v>11.875731999999999</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
-        <v>50984000</v>
+        <v>83000000</v>
       </c>
       <c r="B52" s="1">
-        <v>235.32011</v>
+        <v>147.10462999999999</v>
       </c>
       <c r="C52" s="1">
-        <v>235.32011</v>
+        <v>147.10462999999999</v>
       </c>
       <c r="D52" s="1">
-        <v>11.920685000000001</v>
+        <v>11.894012</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
-        <v>51992000</v>
+        <v>83984000</v>
       </c>
       <c r="B53" s="1">
-        <v>231.21591000000001</v>
+        <v>145.95572000000001</v>
       </c>
       <c r="C53" s="1">
-        <v>231.21591000000001</v>
+        <v>145.95572000000001</v>
       </c>
       <c r="D53" s="1">
-        <v>11.889647999999999</v>
+        <v>11.911407000000001</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
-        <v>53000000</v>
+        <v>84992000</v>
       </c>
       <c r="B54" s="1">
-        <v>227.97833</v>
+        <v>143.84674000000001</v>
       </c>
       <c r="C54" s="1">
-        <v>227.97833</v>
+        <v>143.84674000000001</v>
       </c>
       <c r="D54" s="1">
-        <v>11.858428999999999</v>
+        <v>11.930298000000001</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
-        <v>53988000</v>
+        <v>86000000</v>
       </c>
       <c r="B55" s="1">
-        <v>227.08896999999999</v>
+        <v>145.70195000000001</v>
       </c>
       <c r="C55" s="1">
-        <v>227.08896999999999</v>
+        <v>145.70195000000001</v>
       </c>
       <c r="D55" s="1">
-        <v>11.827728</v>
+        <v>11.950317</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
-        <v>54992000</v>
+        <v>86984000</v>
       </c>
       <c r="B56" s="1">
-        <v>223.51626999999999</v>
+        <v>146.88409999999999</v>
       </c>
       <c r="C56" s="1">
-        <v>223.51626999999999</v>
+        <v>146.88409999999999</v>
       </c>
       <c r="D56" s="1">
-        <v>11.796143000000001</v>
+        <v>11.970276</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
-        <v>56000000</v>
+        <v>87992000</v>
       </c>
       <c r="B57" s="1">
-        <v>219.22086999999999</v>
+        <v>146.21271999999999</v>
       </c>
       <c r="C57" s="1">
-        <v>219.22086999999999</v>
+        <v>146.21271999999999</v>
       </c>
       <c r="D57" s="1">
-        <v>11.764435000000001</v>
+        <v>11.990753</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
-        <v>56984000</v>
+        <v>89000000</v>
       </c>
       <c r="B58" s="1">
-        <v>179.42106999999999</v>
+        <v>147.67114000000001</v>
       </c>
       <c r="C58" s="1">
-        <v>179.42106999999999</v>
+        <v>147.67114000000001</v>
       </c>
       <c r="D58" s="1">
-        <v>11.738007</v>
+        <v>12.011047</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
-        <v>57992000</v>
+        <v>89984000</v>
       </c>
       <c r="B59" s="1">
-        <v>155.28044</v>
+        <v>148.98169999999999</v>
       </c>
       <c r="C59" s="1">
-        <v>155.28044</v>
+        <v>148.98169999999999</v>
       </c>
       <c r="D59" s="1">
-        <v>11.729309000000001</v>
+        <v>12.030792</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
-        <v>59000000</v>
+        <v>90992000</v>
       </c>
       <c r="B60" s="1">
-        <v>148.59575000000001</v>
+        <v>145.78188</v>
       </c>
       <c r="C60" s="1">
-        <v>148.59575000000001</v>
+        <v>145.78188</v>
       </c>
       <c r="D60" s="1">
-        <v>11.730835000000001</v>
+        <v>12.050903</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
-        <v>59984000</v>
+        <v>92000000</v>
       </c>
       <c r="B61" s="1">
-        <v>149.46073999999999</v>
+        <v>153.37633</v>
       </c>
       <c r="C61" s="1">
-        <v>149.46073999999999</v>
+        <v>153.37633</v>
       </c>
       <c r="D61" s="1">
-        <v>11.735412999999999</v>
+        <v>12.0703125</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
-        <v>60992000</v>
+        <v>92988000</v>
       </c>
       <c r="B62" s="1">
-        <v>150.70625000000001</v>
+        <v>181.95935</v>
       </c>
       <c r="C62" s="1">
-        <v>150.70625000000001</v>
+        <v>181.95935</v>
       </c>
       <c r="D62" s="1">
-        <v>11.740662</v>
+        <v>12.076904000000001</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
-        <v>61999999</v>
+        <v>93992000</v>
       </c>
       <c r="B63" s="1">
-        <v>155.40233000000001</v>
+        <v>162.60785000000001</v>
       </c>
       <c r="C63" s="1">
-        <v>155.40233000000001</v>
+        <v>162.60785000000001</v>
       </c>
       <c r="D63" s="1">
-        <v>11.746703999999999</v>
+        <v>12.064575</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
-        <v>62984000</v>
+        <v>95000000</v>
       </c>
       <c r="B64" s="1">
-        <v>159.06612000000001</v>
+        <v>143.74919</v>
       </c>
       <c r="C64" s="1">
-        <v>159.06612000000001</v>
+        <v>143.74919</v>
       </c>
       <c r="D64" s="1">
-        <v>11.754028</v>
+        <v>12.045441</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
-        <v>63992000</v>
+        <v>95988000</v>
       </c>
       <c r="B65" s="1">
-        <v>164.63660999999999</v>
+        <v>143.84100000000001</v>
       </c>
       <c r="C65" s="1">
-        <v>164.63660999999999</v>
+        <v>143.84100000000001</v>
       </c>
       <c r="D65" s="1">
-        <v>11.762207</v>
+        <v>12.039825</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
-        <v>65004000</v>
+        <v>96992000</v>
       </c>
       <c r="B66" s="1">
-        <v>163.52919</v>
+        <v>153.21209999999999</v>
       </c>
       <c r="C66" s="1">
-        <v>163.52919</v>
+        <v>153.21209999999999</v>
       </c>
       <c r="D66" s="1">
-        <v>11.767029000000001</v>
+        <v>12.043945000000001</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
-        <v>65984000</v>
+        <v>98000000</v>
       </c>
       <c r="B67" s="1">
-        <v>152.57642999999999</v>
+        <v>155.46463</v>
       </c>
       <c r="C67" s="1">
-        <v>152.57642999999999</v>
+        <v>155.46463</v>
       </c>
       <c r="D67" s="1">
-        <v>11.765533</v>
+        <v>12.048798</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
-        <v>66992000</v>
+        <v>98984000</v>
       </c>
       <c r="B68" s="1">
-        <v>141.30330000000001</v>
+        <v>157.10641000000001</v>
       </c>
       <c r="C68" s="1">
-        <v>141.30330000000001</v>
+        <v>157.10641000000001</v>
       </c>
       <c r="D68" s="1">
-        <v>11.760192999999999</v>
+        <v>12.051727</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
-        <v>68000000</v>
+        <v>99992000</v>
       </c>
       <c r="B69" s="1">
-        <v>134.60624999999999</v>
+        <v>153.88327000000001</v>
       </c>
       <c r="C69" s="1">
-        <v>134.60624999999999</v>
+        <v>153.88327000000001</v>
       </c>
       <c r="D69" s="1">
-        <v>11.755646</v>
+        <v>12.053284</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
-        <v>68984000</v>
+        <v>101000000</v>
       </c>
       <c r="B70" s="1">
-        <v>133.74315999999999</v>
+        <v>152.41542000000001</v>
       </c>
       <c r="C70" s="1">
-        <v>133.74315999999999</v>
+        <v>152.41542000000001</v>
       </c>
       <c r="D70" s="1">
-        <v>11.753876</v>
+        <v>12.05481</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
-        <v>69992000</v>
+        <v>101984000</v>
       </c>
       <c r="B71" s="1">
-        <v>133.22400999999999</v>
+        <v>153.80238</v>
       </c>
       <c r="C71" s="1">
-        <v>133.22400999999999</v>
+        <v>153.80238</v>
       </c>
       <c r="D71" s="1">
-        <v>11.75412</v>
+        <v>12.056824000000001</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
-        <v>71000000</v>
+        <v>102992000</v>
       </c>
       <c r="B72" s="1">
-        <v>132.66460000000001</v>
+        <v>146.21626000000001</v>
       </c>
       <c r="C72" s="1">
-        <v>132.66460000000001</v>
+        <v>146.21626000000001</v>
       </c>
       <c r="D72" s="1">
-        <v>11.755065999999999</v>
+        <v>12.057159</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
-        <v>71984000</v>
+        <v>104000000</v>
       </c>
       <c r="B73" s="1">
-        <v>135.80251999999999</v>
+        <v>143.29427000000001</v>
       </c>
       <c r="C73" s="1">
-        <v>135.80251999999999</v>
+        <v>143.29427000000001</v>
       </c>
       <c r="D73" s="1">
-        <v>11.755675999999999</v>
+        <v>12.055084000000001</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
-        <v>72992000</v>
+        <v>104984000</v>
       </c>
       <c r="B74" s="1">
-        <v>135.98079000000001</v>
+        <v>139.42067</v>
       </c>
       <c r="C74" s="1">
-        <v>135.98079000000001</v>
+        <v>139.42067</v>
       </c>
       <c r="D74" s="1">
-        <v>11.755737</v>
+        <v>12.051575</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
-        <v>74000000</v>
+        <v>105992000</v>
       </c>
       <c r="B75" s="1">
-        <v>176.97640000000001</v>
+        <v>138.59473</v>
       </c>
       <c r="C75" s="1">
-        <v>176.97640000000001</v>
+        <v>138.59473</v>
       </c>
       <c r="D75" s="1">
-        <v>11.756378</v>
+        <v>12.048980999999999</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
-        <v>74984000</v>
+        <v>107000000</v>
       </c>
       <c r="B76" s="1">
-        <v>189.58678</v>
+        <v>151.11626999999999</v>
       </c>
       <c r="C76" s="1">
-        <v>189.58678</v>
+        <v>151.11626999999999</v>
       </c>
       <c r="D76" s="1">
-        <v>11.754822000000001</v>
+        <v>12.051056000000001</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
-        <v>75992000</v>
+        <v>107984000</v>
       </c>
       <c r="B77" s="1">
-        <v>166.44802999999999</v>
+        <v>173.50429</v>
       </c>
       <c r="C77" s="1">
-        <v>166.44802999999999</v>
+        <v>173.50429</v>
       </c>
       <c r="D77" s="1">
-        <v>11.753204</v>
+        <v>12.061768000000001</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
-        <v>77000000</v>
+        <v>108992000</v>
       </c>
       <c r="B78" s="1">
-        <v>140.12845999999999</v>
+        <v>193.97284999999999</v>
       </c>
       <c r="C78" s="1">
-        <v>140.12845999999999</v>
+        <v>193.97284999999999</v>
       </c>
       <c r="D78" s="1">
-        <v>11.760223</v>
+        <v>12.080933</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
-        <v>77984000</v>
+        <v>110000000</v>
       </c>
       <c r="B79" s="1">
-        <v>140.74431999999999</v>
+        <v>216.56112999999999</v>
       </c>
       <c r="C79" s="1">
-        <v>140.74431999999999</v>
+        <v>216.56112999999999</v>
       </c>
       <c r="D79" s="1">
-        <v>11.780120999999999</v>
+        <v>12.101959000000001</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
-        <v>78992000</v>
+        <v>110984000</v>
       </c>
       <c r="B80" s="1">
-        <v>147.29279</v>
+        <v>226.00272000000001</v>
       </c>
       <c r="C80" s="1">
-        <v>147.29279</v>
+        <v>226.00272000000001</v>
       </c>
       <c r="D80" s="1">
-        <v>11.806854</v>
+        <v>12.121886999999999</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
-        <v>80000000</v>
+        <v>111992000</v>
       </c>
       <c r="B81" s="1">
-        <v>153.44956999999999</v>
+        <v>214.23006000000001</v>
       </c>
       <c r="C81" s="1">
-        <v>153.44956999999999</v>
+        <v>214.23006000000001</v>
       </c>
       <c r="D81" s="1">
-        <v>11.832336</v>
+        <v>12.13147</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
-        <v>80984000</v>
+        <v>113000000</v>
       </c>
       <c r="B82" s="1">
-        <v>156.43575000000001</v>
+        <v>186.31769</v>
       </c>
       <c r="C82" s="1">
-        <v>156.43575000000001</v>
+        <v>186.31769</v>
       </c>
       <c r="D82" s="1">
-        <v>11.855164</v>
+        <v>12.117767000000001</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
-        <v>81992000</v>
+        <v>113984000</v>
       </c>
       <c r="B83" s="1">
-        <v>151.44386</v>
+        <v>164.11375000000001</v>
       </c>
       <c r="C83" s="1">
-        <v>151.44386</v>
+        <v>164.11375000000001</v>
       </c>
       <c r="D83" s="1">
-        <v>11.875731999999999</v>
+        <v>12.097839</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
-        <v>83000000</v>
+        <v>114992000</v>
       </c>
       <c r="B84" s="1">
-        <v>147.10462999999999</v>
+        <v>153.03745000000001</v>
       </c>
       <c r="C84" s="1">
-        <v>147.10462999999999</v>
+        <v>153.03745000000001</v>
       </c>
       <c r="D84" s="1">
-        <v>11.894012</v>
+        <v>12.083800999999999</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
-        <v>83984000</v>
+        <v>116000000</v>
       </c>
       <c r="B85" s="1">
-        <v>145.95572000000001</v>
+        <v>145.39251999999999</v>
       </c>
       <c r="C85" s="1">
-        <v>145.95572000000001</v>
+        <v>145.39251999999999</v>
       </c>
       <c r="D85" s="1">
-        <v>11.911407000000001</v>
+        <v>12.076935000000001</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
-        <v>84992000</v>
+        <v>116984000</v>
       </c>
       <c r="B86" s="1">
-        <v>143.84674000000001</v>
+        <v>138.91417000000001</v>
       </c>
       <c r="C86" s="1">
-        <v>143.84674000000001</v>
+        <v>138.91417000000001</v>
       </c>
       <c r="D86" s="1">
-        <v>11.930298000000001</v>
+        <v>12.072784</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
-        <v>86000000</v>
+        <v>117992000</v>
       </c>
       <c r="B87" s="1">
-        <v>145.70195000000001</v>
+        <v>127.02030000000001</v>
       </c>
       <c r="C87" s="1">
-        <v>145.70195000000001</v>
+        <v>127.02030000000001</v>
       </c>
       <c r="D87" s="1">
-        <v>11.950317</v>
+        <v>12.066742</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
-        <v>86984000</v>
+        <v>119000000</v>
       </c>
       <c r="B88" s="1">
-        <v>146.88409999999999</v>
+        <v>119.37746</v>
       </c>
       <c r="C88" s="1">
-        <v>146.88409999999999</v>
+        <v>119.37746</v>
       </c>
       <c r="D88" s="1">
-        <v>11.970276</v>
+        <v>12.060028000000001</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" s="1">
-        <v>87992000</v>
+        <v>119984000</v>
       </c>
       <c r="B89" s="1">
-        <v>146.21271999999999</v>
+        <v>120.75744</v>
       </c>
       <c r="C89" s="1">
-        <v>146.21271999999999</v>
+        <v>120.75744</v>
       </c>
       <c r="D89" s="1">
-        <v>11.990753</v>
+        <v>12.058472</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" s="1">
-        <v>89000000</v>
+        <v>120992000</v>
       </c>
       <c r="B90" s="1">
-        <v>147.67114000000001</v>
+        <v>124.98492</v>
       </c>
       <c r="C90" s="1">
-        <v>147.67114000000001</v>
+        <v>124.98492</v>
       </c>
       <c r="D90" s="1">
-        <v>12.011047</v>
+        <v>12.060516</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" s="1">
-        <v>89984000</v>
+        <v>122000000</v>
       </c>
       <c r="B91" s="1">
-        <v>148.98169999999999</v>
+        <v>130.55447000000001</v>
       </c>
       <c r="C91" s="1">
-        <v>148.98169999999999</v>
+        <v>130.55447000000001</v>
       </c>
       <c r="D91" s="1">
-        <v>12.030792</v>
+        <v>12.062683</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" s="1">
-        <v>90992000</v>
+        <v>122988000</v>
       </c>
       <c r="B92" s="1">
-        <v>145.78188</v>
+        <v>133.17111</v>
       </c>
       <c r="C92" s="1">
-        <v>145.78188</v>
+        <v>133.17111</v>
       </c>
       <c r="D92" s="1">
-        <v>12.050903</v>
+        <v>12.063843</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" s="1">
-        <v>92000000</v>
+        <v>123992000</v>
       </c>
       <c r="B93" s="1">
-        <v>153.37633</v>
+        <v>138.04678000000001</v>
       </c>
       <c r="C93" s="1">
-        <v>153.37633</v>
+        <v>138.04678000000001</v>
       </c>
       <c r="D93" s="1">
-        <v>12.0703125</v>
+        <v>12.064911</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" s="1">
-        <v>92988000</v>
+        <v>125000000</v>
       </c>
       <c r="B94" s="1">
-        <v>181.95935</v>
+        <v>153.59700000000001</v>
       </c>
       <c r="C94" s="1">
-        <v>181.95935</v>
+        <v>153.59700000000001</v>
       </c>
       <c r="D94" s="1">
-        <v>12.076904000000001</v>
+        <v>12.067963000000001</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" s="1">
-        <v>93992000</v>
+        <v>125983999</v>
       </c>
       <c r="B95" s="1">
-        <v>162.60785000000001</v>
+        <v>163.97364999999999</v>
       </c>
       <c r="C95" s="1">
-        <v>162.60785000000001</v>
+        <v>163.97364999999999</v>
       </c>
       <c r="D95" s="1">
-        <v>12.064575</v>
+        <v>12.073975000000001</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" s="1">
-        <v>95000000</v>
+        <v>126992000</v>
       </c>
       <c r="B96" s="1">
-        <v>143.74919</v>
+        <v>172.40647999999999</v>
       </c>
       <c r="C96" s="1">
-        <v>143.74919</v>
+        <v>172.40647999999999</v>
       </c>
       <c r="D96" s="1">
-        <v>12.045441</v>
+        <v>12.083435</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" s="1">
-        <v>95988000</v>
+        <v>128000000</v>
       </c>
       <c r="B97" s="1">
-        <v>143.84100000000001</v>
+        <v>183.54893000000001</v>
       </c>
       <c r="C97" s="1">
-        <v>143.84100000000001</v>
+        <v>183.54893000000001</v>
       </c>
       <c r="D97" s="1">
-        <v>12.039825</v>
+        <v>12.094970999999999</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" s="1">
-        <v>96992000</v>
+        <v>128988000</v>
       </c>
       <c r="B98" s="1">
-        <v>153.21209999999999</v>
+        <v>194.08398</v>
       </c>
       <c r="C98" s="1">
-        <v>153.21209999999999</v>
+        <v>194.08398</v>
       </c>
       <c r="D98" s="1">
-        <v>12.043945000000001</v>
+        <v>12.105103</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" s="1">
-        <v>98000000</v>
+        <v>129992000</v>
       </c>
       <c r="B99" s="1">
-        <v>155.46463</v>
+        <v>200.19353000000001</v>
       </c>
       <c r="C99" s="1">
-        <v>155.46463</v>
+        <v>200.19353000000001</v>
       </c>
       <c r="D99" s="1">
-        <v>12.048798</v>
+        <v>12.113403</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" s="1">
-        <v>98984000</v>
+        <v>131000000</v>
       </c>
       <c r="B100" s="1">
-        <v>157.10641000000001</v>
+        <v>199.6464</v>
       </c>
       <c r="C100" s="1">
-        <v>157.10641000000001</v>
+        <v>199.6464</v>
       </c>
       <c r="D100" s="1">
-        <v>12.051727</v>
+        <v>12.120331</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" s="1">
-        <v>99992000</v>
+        <v>131984000</v>
       </c>
       <c r="B101" s="1">
-        <v>153.88327000000001</v>
+        <v>191.29532</v>
       </c>
       <c r="C101" s="1">
-        <v>153.88327000000001</v>
+        <v>191.29532</v>
       </c>
       <c r="D101" s="1">
-        <v>12.053284</v>
+        <v>12.123566</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" s="1">
-        <v>101000000</v>
+        <v>132992000</v>
       </c>
       <c r="B102" s="1">
-        <v>152.41542000000001</v>
+        <v>175.21417</v>
       </c>
       <c r="C102" s="1">
-        <v>152.41542000000001</v>
+        <v>175.21417</v>
       </c>
       <c r="D102" s="1">
-        <v>12.05481</v>
+        <v>12.117432000000001</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" s="1">
-        <v>101984000</v>
+        <v>134000000</v>
       </c>
       <c r="B103" s="1">
-        <v>153.80238</v>
+        <v>155.17905999999999</v>
       </c>
       <c r="C103" s="1">
-        <v>153.80238</v>
+        <v>155.17905999999999</v>
       </c>
       <c r="D103" s="1">
-        <v>12.056824000000001</v>
+        <v>12.102631000000001</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" s="1">
-        <v>102992000</v>
+        <v>134984000</v>
       </c>
       <c r="B104" s="1">
-        <v>146.21626000000001</v>
+        <v>138.67586</v>
       </c>
       <c r="C104" s="1">
-        <v>146.21626000000001</v>
+        <v>138.67586</v>
       </c>
       <c r="D104" s="1">
-        <v>12.057159</v>
+        <v>12.0876465</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" s="1">
-        <v>104000000</v>
+        <v>135992000</v>
       </c>
       <c r="B105" s="1">
-        <v>143.29427000000001</v>
+        <v>122.86067</v>
       </c>
       <c r="C105" s="1">
-        <v>143.29427000000001</v>
+        <v>122.86067</v>
       </c>
       <c r="D105" s="1">
-        <v>12.055084000000001</v>
+        <v>12.076202</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" s="1">
-        <v>104984000</v>
+        <v>137004000</v>
       </c>
       <c r="B106" s="1">
-        <v>139.42067</v>
+        <v>113.44347999999999</v>
       </c>
       <c r="C106" s="1">
-        <v>139.42067</v>
+        <v>113.44347999999999</v>
       </c>
       <c r="D106" s="1">
-        <v>12.051575</v>
+        <v>12.067963000000001</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" s="1">
-        <v>105992000</v>
+        <v>137988000</v>
       </c>
       <c r="B107" s="1">
-        <v>138.59473</v>
+        <v>104.85119</v>
       </c>
       <c r="C107" s="1">
-        <v>138.59473</v>
+        <v>104.85119</v>
       </c>
       <c r="D107" s="1">
-        <v>12.048980999999999</v>
+        <v>12.061188</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" s="1">
-        <v>107000000</v>
+        <v>138992000</v>
       </c>
       <c r="B108" s="1">
-        <v>151.11626999999999</v>
+        <v>106.42944</v>
       </c>
       <c r="C108" s="1">
-        <v>151.11626999999999</v>
+        <v>106.42944</v>
       </c>
       <c r="D108" s="1">
-        <v>12.051056000000001</v>
+        <v>12.057617</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" s="1">
-        <v>107984000</v>
+        <v>140000000</v>
       </c>
       <c r="B109" s="1">
-        <v>173.50429</v>
+        <v>111.7634</v>
       </c>
       <c r="C109" s="1">
-        <v>173.50429</v>
+        <v>111.7634</v>
       </c>
       <c r="D109" s="1">
-        <v>12.061768000000001</v>
+        <v>12.058258</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" s="1">
-        <v>108992000</v>
+        <v>140984000</v>
       </c>
       <c r="B110" s="1">
-        <v>193.97284999999999</v>
+        <v>114.470924</v>
       </c>
       <c r="C110" s="1">
-        <v>193.97284999999999</v>
+        <v>114.470924</v>
       </c>
       <c r="D110" s="1">
-        <v>12.080933</v>
+        <v>12.06015</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" s="1">
-        <v>110000000</v>
+        <v>141992000</v>
       </c>
       <c r="B111" s="1">
-        <v>216.56112999999999</v>
+        <v>118.32274</v>
       </c>
       <c r="C111" s="1">
-        <v>216.56112999999999</v>
+        <v>118.32274</v>
       </c>
       <c r="D111" s="1">
-        <v>12.101959000000001</v>
+        <v>12.061432</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" s="1">
-        <v>110984000</v>
+        <v>143000000</v>
       </c>
       <c r="B112" s="1">
-        <v>226.00272000000001</v>
+        <v>123.07172</v>
       </c>
       <c r="C112" s="1">
-        <v>226.00272000000001</v>
+        <v>123.07172</v>
       </c>
       <c r="D112" s="1">
-        <v>12.121886999999999</v>
+        <v>12.061980999999999</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" s="1">
-        <v>111992000</v>
+        <v>143984000</v>
       </c>
       <c r="B113" s="1">
-        <v>214.23006000000001</v>
+        <v>165.83148</v>
       </c>
       <c r="C113" s="1">
-        <v>214.23006000000001</v>
+        <v>165.83148</v>
       </c>
       <c r="D113" s="1">
-        <v>12.13147</v>
+        <v>12.058258</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114" s="1">
-        <v>113000000</v>
+        <v>144992000</v>
       </c>
       <c r="B114" s="1">
-        <v>186.31769</v>
+        <v>155.93625</v>
       </c>
       <c r="C114" s="1">
-        <v>186.31769</v>
+        <v>155.93625</v>
       </c>
       <c r="D114" s="1">
-        <v>12.117767000000001</v>
+        <v>12.053314</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" s="1">
-        <v>113984000</v>
+        <v>146000000</v>
       </c>
       <c r="B115" s="1">
-        <v>164.11375000000001</v>
+        <v>166.54254</v>
       </c>
       <c r="C115" s="1">
-        <v>164.11375000000001</v>
+        <v>166.54254</v>
       </c>
       <c r="D115" s="1">
-        <v>12.097839</v>
+        <v>12.061707</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116" s="1">
-        <v>114992000</v>
+        <v>146988000</v>
       </c>
       <c r="B116" s="1">
-        <v>153.03745000000001</v>
+        <v>186.87866</v>
       </c>
       <c r="C116" s="1">
-        <v>153.03745000000001</v>
+        <v>186.87866</v>
       </c>
       <c r="D116" s="1">
-        <v>12.083800999999999</v>
+        <v>12.077362000000001</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117" s="1">
-        <v>116000000</v>
+        <v>147996000</v>
       </c>
       <c r="B117" s="1">
-        <v>145.39251999999999</v>
+        <v>200.03776999999999</v>
       </c>
       <c r="C117" s="1">
-        <v>145.39251999999999</v>
+        <v>200.03776999999999</v>
       </c>
       <c r="D117" s="1">
-        <v>12.076935000000001</v>
+        <v>12.096283</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" s="1">
-        <v>116984000</v>
+        <v>149000000</v>
       </c>
       <c r="B118" s="1">
-        <v>138.91417000000001</v>
+        <v>189.44076999999999</v>
       </c>
       <c r="C118" s="1">
-        <v>138.91417000000001</v>
+        <v>189.44076999999999</v>
       </c>
       <c r="D118" s="1">
-        <v>12.072784</v>
+        <v>12.106171</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119" s="1">
-        <v>117992000</v>
+        <v>149984000</v>
       </c>
       <c r="B119" s="1">
-        <v>127.02030000000001</v>
+        <v>163.53055000000001</v>
       </c>
       <c r="C119" s="1">
-        <v>127.02030000000001</v>
+        <v>163.53055000000001</v>
       </c>
       <c r="D119" s="1">
-        <v>12.066742</v>
+        <v>12.097899999999999</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120" s="1">
-        <v>119000000</v>
+        <v>150992000</v>
       </c>
       <c r="B120" s="1">
-        <v>119.37746</v>
+        <v>142.64406</v>
       </c>
       <c r="C120" s="1">
-        <v>119.37746</v>
+        <v>142.64406</v>
       </c>
       <c r="D120" s="1">
-        <v>12.060028000000001</v>
+        <v>12.082611</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121" s="1">
-        <v>119984000</v>
+        <v>152000000</v>
       </c>
       <c r="B121" s="1">
-        <v>120.75744</v>
+        <v>133.36315999999999</v>
       </c>
       <c r="C121" s="1">
-        <v>120.75744</v>
+        <v>133.36315999999999</v>
       </c>
       <c r="D121" s="1">
-        <v>12.058472</v>
+        <v>12.07254</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A122" s="1">
-        <v>120992000</v>
+        <v>152984000</v>
       </c>
       <c r="B122" s="1">
-        <v>124.98492</v>
+        <v>136.77238</v>
       </c>
       <c r="C122" s="1">
-        <v>124.98492</v>
+        <v>136.77238</v>
       </c>
       <c r="D122" s="1">
-        <v>12.060516</v>
+        <v>12.070404</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A123" s="1">
-        <v>122000000</v>
+        <v>153992000</v>
       </c>
       <c r="B123" s="1">
-        <v>130.55447000000001</v>
+        <v>142.45274000000001</v>
       </c>
       <c r="C123" s="1">
-        <v>130.55447000000001</v>
+        <v>142.45274000000001</v>
       </c>
       <c r="D123" s="1">
-        <v>12.062683</v>
+        <v>12.072601000000001</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A124" s="1">
-        <v>122988000</v>
+        <v>155000000</v>
       </c>
       <c r="B124" s="1">
-        <v>133.17111</v>
+        <v>144.22005999999999</v>
       </c>
       <c r="C124" s="1">
-        <v>133.17111</v>
+        <v>144.22005999999999</v>
       </c>
       <c r="D124" s="1">
-        <v>12.063843</v>
+        <v>12.074646</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A125" s="1">
-        <v>123992000</v>
+        <v>155984000</v>
       </c>
       <c r="B125" s="1">
-        <v>138.04678000000001</v>
+        <v>144.52181999999999</v>
       </c>
       <c r="C125" s="1">
-        <v>138.04678000000001</v>
+        <v>144.52181999999999</v>
       </c>
       <c r="D125" s="1">
-        <v>12.064911</v>
+        <v>12.074370999999999</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A126" s="1">
-        <v>125000000</v>
+        <v>156992000</v>
       </c>
       <c r="B126" s="1">
-        <v>153.59700000000001</v>
+        <v>140.87816000000001</v>
       </c>
       <c r="C126" s="1">
-        <v>153.59700000000001</v>
+        <v>140.87816000000001</v>
       </c>
       <c r="D126" s="1">
-        <v>12.067963000000001</v>
+        <v>12.071899</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A127" s="1">
-        <v>125983999</v>
+        <v>158000000</v>
       </c>
       <c r="B127" s="1">
-        <v>163.97364999999999</v>
+        <v>135.21906999999999</v>
       </c>
       <c r="C127" s="1">
-        <v>163.97364999999999</v>
+        <v>135.21906999999999</v>
       </c>
       <c r="D127" s="1">
-        <v>12.073975000000001</v>
+        <v>12.068664999999999</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A128" s="1">
-        <v>126992000</v>
+        <v>158984000</v>
       </c>
       <c r="B128" s="1">
-        <v>172.40647999999999</v>
+        <v>131.17475999999999</v>
       </c>
       <c r="C128" s="1">
-        <v>172.40647999999999</v>
+        <v>131.17475999999999</v>
       </c>
       <c r="D128" s="1">
-        <v>12.083435</v>
+        <v>12.064940999999999</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A129" s="1">
-        <v>128000000</v>
+        <v>159992000</v>
       </c>
       <c r="B129" s="1">
-        <v>183.54893000000001</v>
+        <v>121.29705</v>
       </c>
       <c r="C129" s="1">
-        <v>183.54893000000001</v>
+        <v>121.29705</v>
       </c>
       <c r="D129" s="1">
-        <v>12.094970999999999</v>
+        <v>12.059326</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A130" s="1">
-        <v>128988000</v>
+        <v>161000000</v>
       </c>
       <c r="B130" s="1">
-        <v>194.08398</v>
+        <v>109.22356000000001</v>
       </c>
       <c r="C130" s="1">
-        <v>194.08398</v>
+        <v>109.22356000000001</v>
       </c>
       <c r="D130" s="1">
-        <v>12.105103</v>
+        <v>12.058868</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A131" s="1">
-        <v>129992000</v>
+        <v>161984000</v>
       </c>
       <c r="B131" s="1">
-        <v>200.19353000000001</v>
+        <v>149.14510000000001</v>
       </c>
       <c r="C131" s="1">
-        <v>200.19353000000001</v>
+        <v>149.14510000000001</v>
       </c>
       <c r="D131" s="1">
-        <v>12.113403</v>
+        <v>12.064147999999999</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A132" s="1">
-        <v>131000000</v>
+        <v>162992000</v>
       </c>
       <c r="B132" s="1">
-        <v>199.6464</v>
+        <v>167.25919999999999</v>
       </c>
       <c r="C132" s="1">
-        <v>199.6464</v>
+        <v>167.25919999999999</v>
       </c>
       <c r="D132" s="1">
-        <v>12.120331</v>
+        <v>12.065429999999999</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A133" s="1">
-        <v>131984000</v>
+        <v>164000000</v>
       </c>
       <c r="B133" s="1">
-        <v>191.29532</v>
+        <v>181.87807000000001</v>
       </c>
       <c r="C133" s="1">
-        <v>191.29532</v>
+        <v>181.87807000000001</v>
       </c>
       <c r="D133" s="1">
-        <v>12.123566</v>
+        <v>12.066589</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A134" s="1">
-        <v>132992000</v>
+        <v>164984000</v>
       </c>
       <c r="B134" s="1">
-        <v>175.21417</v>
+        <v>186.64867000000001</v>
       </c>
       <c r="C134" s="1">
-        <v>175.21417</v>
+        <v>186.64867000000001</v>
       </c>
       <c r="D134" s="1">
-        <v>12.117432000000001</v>
+        <v>12.067932000000001</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A135" s="1">
-        <v>134000000</v>
+        <v>165996000</v>
       </c>
       <c r="B135" s="1">
-        <v>155.17905999999999</v>
+        <v>181.57416000000001</v>
       </c>
       <c r="C135" s="1">
-        <v>155.17905999999999</v>
+        <v>181.57416000000001</v>
       </c>
       <c r="D135" s="1">
-        <v>12.102631000000001</v>
+        <v>12.068909</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A136" s="1">
-        <v>134984000</v>
+        <v>167000000</v>
       </c>
       <c r="B136" s="1">
-        <v>138.67586</v>
+        <v>165.81233</v>
       </c>
       <c r="C136" s="1">
-        <v>138.67586</v>
+        <v>165.81233</v>
       </c>
       <c r="D136" s="1">
-        <v>12.0876465</v>
+        <v>12.066284</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A137" s="1">
-        <v>135992000</v>
+        <v>167988000</v>
       </c>
       <c r="B137" s="1">
-        <v>122.86067</v>
+        <v>151.57004000000001</v>
       </c>
       <c r="C137" s="1">
-        <v>122.86067</v>
+        <v>151.57004000000001</v>
       </c>
       <c r="D137" s="1">
-        <v>12.076202</v>
+        <v>12.058075000000001</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A138" s="1">
-        <v>137004000</v>
+        <v>168992000</v>
       </c>
       <c r="B138" s="1">
-        <v>113.44347999999999</v>
+        <v>119.07810000000001</v>
       </c>
       <c r="C138" s="1">
-        <v>113.44347999999999</v>
+        <v>119.07810000000001</v>
       </c>
       <c r="D138" s="1">
-        <v>12.067963000000001</v>
+        <v>12.048553</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A139" s="1">
-        <v>137988000</v>
+        <v>170000000</v>
       </c>
       <c r="B139" s="1">
-        <v>104.85119</v>
+        <v>94.736689999999996</v>
       </c>
       <c r="C139" s="1">
-        <v>104.85119</v>
+        <v>94.736689999999996</v>
       </c>
       <c r="D139" s="1">
-        <v>12.061188</v>
+        <v>12.044891</v>
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A140" s="1">
-        <v>138992000</v>
+        <v>170988000</v>
       </c>
       <c r="B140" s="1">
-        <v>106.42944</v>
+        <v>90.488190000000003</v>
       </c>
       <c r="C140" s="1">
-        <v>106.42944</v>
+        <v>90.488190000000003</v>
       </c>
       <c r="D140" s="1">
-        <v>12.057617</v>
+        <v>12.050446000000001</v>
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A141" s="1">
-        <v>140000000</v>
+        <v>171996000</v>
       </c>
       <c r="B141" s="1">
-        <v>111.7634</v>
+        <v>94.189930000000004</v>
       </c>
       <c r="C141" s="1">
-        <v>111.7634</v>
+        <v>94.189930000000004</v>
       </c>
       <c r="D141" s="1">
-        <v>12.058258</v>
+        <v>12.060059000000001</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A142" s="1">
-        <v>140984000</v>
+        <v>173000000</v>
       </c>
       <c r="B142" s="1">
-        <v>114.470924</v>
+        <v>98.939064000000002</v>
       </c>
       <c r="C142" s="1">
-        <v>114.470924</v>
+        <v>98.939064000000002</v>
       </c>
       <c r="D142" s="1">
-        <v>12.06015</v>
+        <v>12.067902</v>
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A143" s="1">
-        <v>141992000</v>
+        <v>173984000</v>
       </c>
       <c r="B143" s="1">
-        <v>118.32274</v>
+        <v>96.551575</v>
       </c>
       <c r="C143" s="1">
-        <v>118.32274</v>
+        <v>96.551575</v>
       </c>
       <c r="D143" s="1">
-        <v>12.061432</v>
+        <v>12.071899</v>
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A144" s="1">
-        <v>143000000</v>
+        <v>174996000</v>
       </c>
       <c r="B144" s="1">
-        <v>123.07172</v>
+        <v>94.413330000000002</v>
       </c>
       <c r="C144" s="1">
-        <v>123.07172</v>
+        <v>94.413330000000002</v>
       </c>
       <c r="D144" s="1">
-        <v>12.061980999999999</v>
+        <v>12.073242</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A145" s="1">
-        <v>143984000</v>
+        <v>176000000</v>
       </c>
       <c r="B145" s="1">
-        <v>165.83148</v>
+        <v>85.354740000000007</v>
       </c>
       <c r="C145" s="1">
-        <v>165.83148</v>
+        <v>85.354740000000007</v>
       </c>
       <c r="D145" s="1">
-        <v>12.058258</v>
+        <v>12.071777000000001</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A146" s="1">
-        <v>144992000</v>
+        <v>176984000</v>
       </c>
       <c r="B146" s="1">
-        <v>155.93625</v>
+        <v>74.103309999999993</v>
       </c>
       <c r="C146" s="1">
-        <v>155.93625</v>
+        <v>74.103309999999993</v>
       </c>
       <c r="D146" s="1">
-        <v>12.053314</v>
+        <v>12.078979500000001</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A147" s="1">
-        <v>146000000</v>
+        <v>177992000</v>
       </c>
       <c r="B147" s="1">
-        <v>166.54254</v>
+        <v>80.904960000000003</v>
       </c>
       <c r="C147" s="1">
-        <v>166.54254</v>
+        <v>80.904960000000003</v>
       </c>
       <c r="D147" s="1">
-        <v>12.061707</v>
+        <v>12.097229</v>
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A148" s="1">
-        <v>146988000</v>
+        <v>179004000</v>
       </c>
       <c r="B148" s="1">
-        <v>186.87866</v>
+        <v>88.917990000000003</v>
       </c>
       <c r="C148" s="1">
-        <v>186.87866</v>
+        <v>88.917990000000003</v>
       </c>
       <c r="D148" s="1">
-        <v>12.077362000000001</v>
+        <v>12.116790999999999</v>
       </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A149" s="1">
-        <v>147996000</v>
+        <v>179984000</v>
       </c>
       <c r="B149" s="1">
-        <v>200.03776999999999</v>
+        <v>84.679053999999994</v>
       </c>
       <c r="C149" s="1">
-        <v>200.03776999999999</v>
+        <v>84.679053999999994</v>
       </c>
       <c r="D149" s="1">
-        <v>12.096283</v>
+        <v>12.131714000000001</v>
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A150" s="1">
-        <v>149000000</v>
+        <v>180996000</v>
       </c>
       <c r="B150" s="1">
-        <v>189.44076999999999</v>
+        <v>79.429990000000004</v>
       </c>
       <c r="C150" s="1">
-        <v>189.44076999999999</v>
+        <v>79.429990000000004</v>
       </c>
       <c r="D150" s="1">
-        <v>12.106171</v>
+        <v>12.143981999999999</v>
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A151" s="1">
-        <v>149984000</v>
+        <v>182004000</v>
       </c>
       <c r="B151" s="1">
-        <v>163.53055000000001</v>
+        <v>75.748795000000001</v>
       </c>
       <c r="C151" s="1">
-        <v>163.53055000000001</v>
+        <v>75.748795000000001</v>
       </c>
       <c r="D151" s="1">
-        <v>12.097899999999999</v>
+        <v>12.155975</v>
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A152" s="1">
-        <v>150992000</v>
+        <v>182988000</v>
       </c>
       <c r="B152" s="1">
-        <v>142.64406</v>
+        <v>72.524445</v>
       </c>
       <c r="C152" s="1">
-        <v>142.64406</v>
+        <v>72.524445</v>
       </c>
       <c r="D152" s="1">
-        <v>12.082611</v>
+        <v>12.168120999999999</v>
       </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A153" s="1">
-        <v>152000000</v>
+        <v>183992000</v>
       </c>
       <c r="B153" s="1">
-        <v>133.36315999999999</v>
+        <v>72.975549999999998</v>
       </c>
       <c r="C153" s="1">
-        <v>133.36315999999999</v>
+        <v>72.975549999999998</v>
       </c>
       <c r="D153" s="1">
-        <v>12.07254</v>
+        <v>12.180237</v>
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A154" s="1">
-        <v>152984000</v>
+        <v>185000000</v>
       </c>
       <c r="B154" s="1">
-        <v>136.77238</v>
+        <v>71.558875999999998</v>
       </c>
       <c r="C154" s="1">
-        <v>136.77238</v>
+        <v>71.558875999999998</v>
       </c>
       <c r="D154" s="1">
-        <v>12.070404</v>
+        <v>12.191406000000001</v>
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A155" s="1">
-        <v>153992000</v>
+        <v>185988000</v>
       </c>
       <c r="B155" s="1">
-        <v>142.45274000000001</v>
+        <v>68.76737</v>
       </c>
       <c r="C155" s="1">
-        <v>142.45274000000001</v>
+        <v>68.76737</v>
       </c>
       <c r="D155" s="1">
-        <v>12.072601000000001</v>
+        <v>12.201568999999999</v>
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A156" s="1">
-        <v>155000000</v>
+        <v>186996000</v>
       </c>
       <c r="B156" s="1">
-        <v>144.22005999999999</v>
+        <v>68.763909999999996</v>
       </c>
       <c r="C156" s="1">
-        <v>144.22005999999999</v>
+        <v>68.763909999999996</v>
       </c>
       <c r="D156" s="1">
-        <v>12.074646</v>
+        <v>12.211548000000001</v>
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A157" s="1">
-        <v>155984000</v>
+        <v>188000000</v>
       </c>
       <c r="B157" s="1">
-        <v>144.52181999999999</v>
+        <v>67.600944999999996</v>
       </c>
       <c r="C157" s="1">
-        <v>144.52181999999999</v>
+        <v>67.600944999999996</v>
       </c>
       <c r="D157" s="1">
-        <v>12.074370999999999</v>
+        <v>12.221007999999999</v>
       </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A158" s="1">
-        <v>156992000</v>
+        <v>188984000</v>
       </c>
       <c r="B158" s="1">
-        <v>140.87816000000001</v>
+        <v>67.199259999999995</v>
       </c>
       <c r="C158" s="1">
-        <v>140.87816000000001</v>
+        <v>67.199259999999995</v>
       </c>
       <c r="D158" s="1">
-        <v>12.071899</v>
+        <v>12.230193999999999</v>
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A159" s="1">
-        <v>158000000</v>
+        <v>189996000</v>
       </c>
       <c r="B159" s="1">
-        <v>135.21906999999999</v>
+        <v>66.948070000000001</v>
       </c>
       <c r="C159" s="1">
-        <v>135.21906999999999</v>
+        <v>66.948070000000001</v>
       </c>
       <c r="D159" s="1">
-        <v>12.068664999999999</v>
+        <v>12.23996</v>
       </c>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A160" s="1">
-        <v>158984000</v>
+        <v>191000000</v>
       </c>
       <c r="B160" s="1">
-        <v>131.17475999999999</v>
+        <v>66.911450000000002</v>
       </c>
       <c r="C160" s="1">
-        <v>131.17475999999999</v>
+        <v>66.911450000000002</v>
       </c>
       <c r="D160" s="1">
-        <v>12.064940999999999</v>
+        <v>12.249817</v>
       </c>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A161" s="1">
-        <v>159992000</v>
+        <v>191984000</v>
       </c>
       <c r="B161" s="1">
-        <v>121.29705</v>
+        <v>66.545203999999998</v>
       </c>
       <c r="C161" s="1">
-        <v>121.29705</v>
+        <v>66.545203999999998</v>
       </c>
       <c r="D161" s="1">
-        <v>12.059326</v>
+        <v>12.259124999999999</v>
       </c>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A162" s="1">
-        <v>161000000</v>
+        <v>192996000</v>
       </c>
       <c r="B162" s="1">
-        <v>109.22356000000001</v>
+        <v>66.107740000000007</v>
       </c>
       <c r="C162" s="1">
-        <v>109.22356000000001</v>
+        <v>66.107740000000007</v>
       </c>
       <c r="D162" s="1">
-        <v>12.058868</v>
+        <v>12.268340999999999</v>
       </c>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A163" s="1">
-        <v>161984000</v>
+        <v>194000000</v>
       </c>
       <c r="B163" s="1">
-        <v>149.14510000000001</v>
+        <v>66.941839999999999</v>
       </c>
       <c r="C163" s="1">
-        <v>149.14510000000001</v>
+        <v>66.941839999999999</v>
       </c>
       <c r="D163" s="1">
-        <v>12.064147999999999</v>
+        <v>12.277466</v>
       </c>
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A164" s="1">
-        <v>162992000</v>
+        <v>194984000</v>
       </c>
       <c r="B164" s="1">
-        <v>167.25919999999999</v>
+        <v>67.913910000000001</v>
       </c>
       <c r="C164" s="1">
-        <v>167.25919999999999</v>
+        <v>67.913910000000001</v>
       </c>
       <c r="D164" s="1">
-        <v>12.065429999999999</v>
+        <v>12.286652</v>
       </c>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A165" s="1">
-        <v>164000000</v>
+        <v>195992000</v>
       </c>
       <c r="B165" s="1">
-        <v>181.87807000000001</v>
+        <v>67.192700000000002</v>
       </c>
       <c r="C165" s="1">
-        <v>181.87807000000001</v>
+        <v>67.192700000000002</v>
       </c>
       <c r="D165" s="1">
-        <v>12.066589</v>
+        <v>12.296355999999999</v>
       </c>
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A166" s="1">
-        <v>164984000</v>
+        <v>197000000</v>
       </c>
       <c r="B166" s="1">
-        <v>186.64867000000001</v>
+        <v>67.944109999999995</v>
       </c>
       <c r="C166" s="1">
-        <v>186.64867000000001</v>
+        <v>67.944109999999995</v>
       </c>
       <c r="D166" s="1">
-        <v>12.067932000000001</v>
+        <v>12.306061</v>
       </c>
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A167" s="1">
-        <v>165996000</v>
+        <v>197984000</v>
       </c>
       <c r="B167" s="1">
-        <v>181.57416000000001</v>
+        <v>67.124825000000001</v>
       </c>
       <c r="C167" s="1">
-        <v>181.57416000000001</v>
+        <v>67.124825000000001</v>
       </c>
       <c r="D167" s="1">
-        <v>12.068909</v>
+        <v>12.315246999999999</v>
       </c>
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A168" s="1">
-        <v>167000000</v>
+        <v>198996000</v>
       </c>
       <c r="B168" s="1">
-        <v>165.81233</v>
+        <v>68.0351</v>
       </c>
       <c r="C168" s="1">
-        <v>165.81233</v>
+        <v>68.0351</v>
       </c>
       <c r="D168" s="1">
-        <v>12.066284</v>
+        <v>12.324463</v>
       </c>
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A169" s="1">
-        <v>167988000</v>
+        <v>200000000</v>
       </c>
       <c r="B169" s="1">
-        <v>151.57004000000001</v>
+        <v>66.99427</v>
       </c>
       <c r="C169" s="1">
-        <v>151.57004000000001</v>
+        <v>66.99427</v>
       </c>
       <c r="D169" s="1">
-        <v>12.058075000000001</v>
+        <v>12.333983999999999</v>
       </c>
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A170" s="1">
-        <v>168992000</v>
+        <v>200984000</v>
       </c>
       <c r="B170" s="1">
-        <v>119.07810000000001</v>
+        <v>69.293976000000001</v>
       </c>
       <c r="C170" s="1">
-        <v>119.07810000000001</v>
+        <v>69.293976000000001</v>
       </c>
       <c r="D170" s="1">
-        <v>12.048553</v>
+        <v>12.343902999999999</v>
       </c>
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A171" s="1">
-        <v>170000000</v>
+        <v>201992000</v>
       </c>
       <c r="B171" s="1">
-        <v>94.736689999999996</v>
+        <v>70.31071</v>
       </c>
       <c r="C171" s="1">
-        <v>94.736689999999996</v>
+        <v>70.31071</v>
       </c>
       <c r="D171" s="1">
-        <v>12.044891</v>
+        <v>12.354004</v>
       </c>
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A172" s="1">
-        <v>170988000</v>
+        <v>203000000</v>
       </c>
       <c r="B172" s="1">
-        <v>90.488190000000003</v>
+        <v>67.094160000000002</v>
       </c>
       <c r="C172" s="1">
-        <v>90.488190000000003</v>
+        <v>67.094160000000002</v>
       </c>
       <c r="D172" s="1">
-        <v>12.050446000000001</v>
+        <v>12.363586</v>
       </c>
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A173" s="1">
-        <v>171996000</v>
+        <v>203984000</v>
       </c>
       <c r="B173" s="1">
-        <v>94.189930000000004</v>
+        <v>67.854299999999995</v>
       </c>
       <c r="C173" s="1">
-        <v>94.189930000000004</v>
+        <v>67.854299999999995</v>
       </c>
       <c r="D173" s="1">
-        <v>12.060059000000001</v>
+        <v>12.372559000000001</v>
       </c>
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A174" s="1">
-        <v>173000000</v>
+        <v>204996000</v>
       </c>
       <c r="B174" s="1">
-        <v>98.939064000000002</v>
+        <v>66.73724</v>
       </c>
       <c r="C174" s="1">
-        <v>98.939064000000002</v>
+        <v>66.73724</v>
       </c>
       <c r="D174" s="1">
-        <v>12.067902</v>
+        <v>12.381866</v>
       </c>
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A175" s="1">
-        <v>173984000</v>
+        <v>206004000</v>
       </c>
       <c r="B175" s="1">
-        <v>96.551575</v>
+        <v>65.913240000000002</v>
       </c>
       <c r="C175" s="1">
-        <v>96.551575</v>
+        <v>65.913240000000002</v>
       </c>
       <c r="D175" s="1">
-        <v>12.071899</v>
+        <v>12.392455999999999</v>
       </c>
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A176" s="1">
-        <v>174996000</v>
+        <v>206988000</v>
       </c>
       <c r="B176" s="1">
-        <v>94.413330000000002</v>
+        <v>17.514620000000001</v>
       </c>
       <c r="C176" s="1">
-        <v>94.413330000000002</v>
+        <v>17.514620000000001</v>
       </c>
       <c r="D176" s="1">
-        <v>12.073242</v>
+        <v>12.404602000000001</v>
       </c>
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A177" s="1">
-        <v>176000000</v>
+        <v>207996000</v>
       </c>
       <c r="B177" s="1">
-        <v>85.354740000000007</v>
+        <v>1.4810251999999999</v>
       </c>
       <c r="C177" s="1">
-        <v>85.354740000000007</v>
+        <v>1.4810251999999999</v>
       </c>
       <c r="D177" s="1">
-        <v>12.071777000000001</v>
+        <v>12.404602000000001</v>
       </c>
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A178" s="1">
-        <v>176984000</v>
+        <v>209000000</v>
       </c>
       <c r="B178" s="1">
-        <v>74.103309999999993</v>
+        <v>1.2954121000000001</v>
       </c>
       <c r="C178" s="1">
-        <v>74.103309999999993</v>
+        <v>1.2954121000000001</v>
       </c>
       <c r="D178" s="1">
-        <v>12.078979500000001</v>
+        <v>12.404602000000001</v>
       </c>
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A179" s="1">
-        <v>177992000</v>
+        <v>209984000</v>
       </c>
       <c r="B179" s="1">
-        <v>80.904960000000003</v>
+        <v>1.9000417999999999</v>
       </c>
       <c r="C179" s="1">
-        <v>80.904960000000003</v>
+        <v>1.9000417999999999</v>
       </c>
       <c r="D179" s="1">
-        <v>12.097229</v>
+        <v>12.404602000000001</v>
       </c>
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A180" s="1">
-        <v>179004000</v>
+        <v>210996000</v>
       </c>
       <c r="B180" s="1">
-        <v>88.917990000000003</v>
+        <v>0.83838520000000005</v>
       </c>
       <c r="C180" s="1">
-        <v>88.917990000000003</v>
+        <v>0.83838520000000005</v>
       </c>
       <c r="D180" s="1">
-        <v>12.116790999999999</v>
-      </c>
-    </row>
-    <row r="181" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A181" s="1">
-        <v>179984000</v>
-      </c>
-      <c r="B181" s="1">
-        <v>84.679053999999994</v>
-      </c>
-      <c r="C181" s="1">
-        <v>84.679053999999994</v>
-      </c>
-      <c r="D181" s="1">
-        <v>12.131714000000001</v>
-      </c>
-    </row>
-    <row r="182" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A182" s="1">
-        <v>180996000</v>
-      </c>
-      <c r="B182" s="1">
-        <v>79.429990000000004</v>
-      </c>
-      <c r="C182" s="1">
-        <v>79.429990000000004</v>
-      </c>
-      <c r="D182" s="1">
-        <v>12.143981999999999</v>
-      </c>
-    </row>
-    <row r="183" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A183" s="1">
-        <v>182004000</v>
-      </c>
-      <c r="B183" s="1">
-        <v>75.748795000000001</v>
-      </c>
-      <c r="C183" s="1">
-        <v>75.748795000000001</v>
-      </c>
-      <c r="D183" s="1">
-        <v>12.155975</v>
-      </c>
-    </row>
-    <row r="184" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A184" s="1">
-        <v>182988000</v>
-      </c>
-      <c r="B184" s="1">
-        <v>72.524445</v>
-      </c>
-      <c r="C184" s="1">
-        <v>72.524445</v>
-      </c>
-      <c r="D184" s="1">
-        <v>12.168120999999999</v>
-      </c>
-    </row>
-    <row r="185" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A185" s="1">
-        <v>183992000</v>
-      </c>
-      <c r="B185" s="1">
-        <v>72.975549999999998</v>
-      </c>
-      <c r="C185" s="1">
-        <v>72.975549999999998</v>
-      </c>
-      <c r="D185" s="1">
-        <v>12.180237</v>
-      </c>
-    </row>
-    <row r="186" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A186" s="1">
-        <v>185000000</v>
-      </c>
-      <c r="B186" s="1">
-        <v>71.558875999999998</v>
-      </c>
-      <c r="C186" s="1">
-        <v>71.558875999999998</v>
-      </c>
-      <c r="D186" s="1">
-        <v>12.191406000000001</v>
-      </c>
-    </row>
-    <row r="187" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A187" s="1">
-        <v>185988000</v>
-      </c>
-      <c r="B187" s="1">
-        <v>68.76737</v>
-      </c>
-      <c r="C187" s="1">
-        <v>68.76737</v>
-      </c>
-      <c r="D187" s="1">
-        <v>12.201568999999999</v>
-      </c>
-    </row>
-    <row r="188" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A188" s="1">
-        <v>186996000</v>
-      </c>
-      <c r="B188" s="1">
-        <v>68.763909999999996</v>
-      </c>
-      <c r="C188" s="1">
-        <v>68.763909999999996</v>
-      </c>
-      <c r="D188" s="1">
-        <v>12.211548000000001</v>
-      </c>
-    </row>
-    <row r="189" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A189" s="1">
-        <v>188000000</v>
-      </c>
-      <c r="B189" s="1">
-        <v>67.600944999999996</v>
-      </c>
-      <c r="C189" s="1">
-        <v>67.600944999999996</v>
-      </c>
-      <c r="D189" s="1">
-        <v>12.221007999999999</v>
-      </c>
-    </row>
-    <row r="190" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A190" s="1">
-        <v>188984000</v>
-      </c>
-      <c r="B190" s="1">
-        <v>67.199259999999995</v>
-      </c>
-      <c r="C190" s="1">
-        <v>67.199259999999995</v>
-      </c>
-      <c r="D190" s="1">
-        <v>12.230193999999999</v>
-      </c>
-    </row>
-    <row r="191" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A191" s="1">
-        <v>189996000</v>
-      </c>
-      <c r="B191" s="1">
-        <v>66.948070000000001</v>
-      </c>
-      <c r="C191" s="1">
-        <v>66.948070000000001</v>
-      </c>
-      <c r="D191" s="1">
-        <v>12.23996</v>
-      </c>
-    </row>
-    <row r="192" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A192" s="1">
-        <v>191000000</v>
-      </c>
-      <c r="B192" s="1">
-        <v>66.911450000000002</v>
-      </c>
-      <c r="C192" s="1">
-        <v>66.911450000000002</v>
-      </c>
-      <c r="D192" s="1">
-        <v>12.249817</v>
-      </c>
-    </row>
-    <row r="193" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A193" s="1">
-        <v>191984000</v>
-      </c>
-      <c r="B193" s="1">
-        <v>66.545203999999998</v>
-      </c>
-      <c r="C193" s="1">
-        <v>66.545203999999998</v>
-      </c>
-      <c r="D193" s="1">
-        <v>12.259124999999999</v>
-      </c>
-    </row>
-    <row r="194" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A194" s="1">
-        <v>192996000</v>
-      </c>
-      <c r="B194" s="1">
-        <v>66.107740000000007</v>
-      </c>
-      <c r="C194" s="1">
-        <v>66.107740000000007</v>
-      </c>
-      <c r="D194" s="1">
-        <v>12.268340999999999</v>
-      </c>
-    </row>
-    <row r="195" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A195" s="1">
-        <v>194000000</v>
-      </c>
-      <c r="B195" s="1">
-        <v>66.941839999999999</v>
-      </c>
-      <c r="C195" s="1">
-        <v>66.941839999999999</v>
-      </c>
-      <c r="D195" s="1">
-        <v>12.277466</v>
-      </c>
-    </row>
-    <row r="196" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A196" s="1">
-        <v>194984000</v>
-      </c>
-      <c r="B196" s="1">
-        <v>67.913910000000001</v>
-      </c>
-      <c r="C196" s="1">
-        <v>67.913910000000001</v>
-      </c>
-      <c r="D196" s="1">
-        <v>12.286652</v>
-      </c>
-    </row>
-    <row r="197" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A197" s="1">
-        <v>195992000</v>
-      </c>
-      <c r="B197" s="1">
-        <v>67.192700000000002</v>
-      </c>
-      <c r="C197" s="1">
-        <v>67.192700000000002</v>
-      </c>
-      <c r="D197" s="1">
-        <v>12.296355999999999</v>
-      </c>
-    </row>
-    <row r="198" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A198" s="1">
-        <v>197000000</v>
-      </c>
-      <c r="B198" s="1">
-        <v>67.944109999999995</v>
-      </c>
-      <c r="C198" s="1">
-        <v>67.944109999999995</v>
-      </c>
-      <c r="D198" s="1">
-        <v>12.306061</v>
-      </c>
-    </row>
-    <row r="199" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A199" s="1">
-        <v>197984000</v>
-      </c>
-      <c r="B199" s="1">
-        <v>67.124825000000001</v>
-      </c>
-      <c r="C199" s="1">
-        <v>67.124825000000001</v>
-      </c>
-      <c r="D199" s="1">
-        <v>12.315246999999999</v>
-      </c>
-    </row>
-    <row r="200" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A200" s="1">
-        <v>198996000</v>
-      </c>
-      <c r="B200" s="1">
-        <v>68.0351</v>
-      </c>
-      <c r="C200" s="1">
-        <v>68.0351</v>
-      </c>
-      <c r="D200" s="1">
-        <v>12.324463</v>
-      </c>
-    </row>
-    <row r="201" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A201" s="1">
-        <v>200000000</v>
-      </c>
-      <c r="B201" s="1">
-        <v>66.99427</v>
-      </c>
-      <c r="C201" s="1">
-        <v>66.99427</v>
-      </c>
-      <c r="D201" s="1">
-        <v>12.333983999999999</v>
-      </c>
-    </row>
-    <row r="202" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A202" s="1">
-        <v>200984000</v>
-      </c>
-      <c r="B202" s="1">
-        <v>69.293976000000001</v>
-      </c>
-      <c r="C202" s="1">
-        <v>69.293976000000001</v>
-      </c>
-      <c r="D202" s="1">
-        <v>12.343902999999999</v>
-      </c>
-    </row>
-    <row r="203" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A203" s="1">
-        <v>201992000</v>
-      </c>
-      <c r="B203" s="1">
-        <v>70.31071</v>
-      </c>
-      <c r="C203" s="1">
-        <v>70.31071</v>
-      </c>
-      <c r="D203" s="1">
-        <v>12.354004</v>
-      </c>
-    </row>
-    <row r="204" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A204" s="1">
-        <v>203000000</v>
-      </c>
-      <c r="B204" s="1">
-        <v>67.094160000000002</v>
-      </c>
-      <c r="C204" s="1">
-        <v>67.094160000000002</v>
-      </c>
-      <c r="D204" s="1">
-        <v>12.363586</v>
-      </c>
-    </row>
-    <row r="205" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A205" s="1">
-        <v>203984000</v>
-      </c>
-      <c r="B205" s="1">
-        <v>67.854299999999995</v>
-      </c>
-      <c r="C205" s="1">
-        <v>67.854299999999995</v>
-      </c>
-      <c r="D205" s="1">
-        <v>12.372559000000001</v>
-      </c>
-    </row>
-    <row r="206" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A206" s="1">
-        <v>204996000</v>
-      </c>
-      <c r="B206" s="1">
-        <v>66.73724</v>
-      </c>
-      <c r="C206" s="1">
-        <v>66.73724</v>
-      </c>
-      <c r="D206" s="1">
-        <v>12.381866</v>
-      </c>
-    </row>
-    <row r="207" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A207" s="1">
-        <v>206004000</v>
-      </c>
-      <c r="B207" s="1">
-        <v>65.913240000000002</v>
-      </c>
-      <c r="C207" s="1">
-        <v>65.913240000000002</v>
-      </c>
-      <c r="D207" s="1">
-        <v>12.392455999999999</v>
-      </c>
-    </row>
-    <row r="208" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A208" s="1">
-        <v>206988000</v>
-      </c>
-      <c r="B208" s="1">
-        <v>17.514620000000001</v>
-      </c>
-      <c r="C208" s="1">
-        <v>17.514620000000001</v>
-      </c>
-      <c r="D208" s="1">
-        <v>12.404602000000001</v>
-      </c>
-    </row>
-    <row r="209" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A209" s="1">
-        <v>207996000</v>
-      </c>
-      <c r="B209" s="1">
-        <v>1.4810251999999999</v>
-      </c>
-      <c r="C209" s="1">
-        <v>1.4810251999999999</v>
-      </c>
-      <c r="D209" s="1">
-        <v>12.404602000000001</v>
-      </c>
-    </row>
-    <row r="210" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A210" s="1">
-        <v>209000000</v>
-      </c>
-      <c r="B210" s="1">
-        <v>1.2954121000000001</v>
-      </c>
-      <c r="C210" s="1">
-        <v>1.2954121000000001</v>
-      </c>
-      <c r="D210" s="1">
-        <v>12.404602000000001</v>
-      </c>
-    </row>
-    <row r="211" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A211" s="1">
-        <v>209984000</v>
-      </c>
-      <c r="B211" s="1">
-        <v>1.9000417999999999</v>
-      </c>
-      <c r="C211" s="1">
-        <v>1.9000417999999999</v>
-      </c>
-      <c r="D211" s="1">
-        <v>12.404602000000001</v>
-      </c>
-    </row>
-    <row r="212" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A212" s="1">
-        <v>210996000</v>
-      </c>
-      <c r="B212" s="1">
-        <v>0.83838520000000005</v>
-      </c>
-      <c r="C212" s="1">
-        <v>0.83838520000000005</v>
-      </c>
-      <c r="D212" s="1">
         <v>12.404602000000001</v>
       </c>
     </row>

</xml_diff>